<commit_message>
Upgraded to Windows Project
</commit_message>
<xml_diff>
--- a/Processes/CreateEmployeeReport/Report.xlsx
+++ b/Processes/CreateEmployeeReport/Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anubhav shankar\OneDrive - UiPath\Enablement\Integrations\Workday\WKDY_EmployeeReport\Processes\CreateEmployeeReport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\WKDY_EmployeeReport\Processes\CreateEmployeeReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6EE6CE-AA58-44A4-B6E1-A42ABE696C9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542B6662-905D-46E8-88D2-7B6B2C0F35C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4640" windowWidth="3790" windowHeight="1450" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="3" r:id="rId1"/>
@@ -1194,16 +1194,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6254,21 +6254,21 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -6308,7 +6308,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -6356,7 +6356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -6372,10 +6372,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>200000</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>100000</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>200000</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>1200000</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>1800000</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>300000</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>4</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>200000</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>100000</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>300000</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>10</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>100000</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>200000</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>200000</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>100000</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>3</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>200000</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>500000</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>300000</v>
       </c>
@@ -6567,7 +6567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>200000</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>100000</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>500000</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>400000</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>0</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>400000</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>200000</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>14</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>200000</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>25</v>
       </c>
@@ -6677,18 +6677,18 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.36328125" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" customWidth="1"/>
-    <col min="3" max="3" width="50.26953125" customWidth="1"/>
-    <col min="4" max="4" width="31.81640625" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="64" customWidth="1"/>
-    <col min="12" max="12" width="17.08984375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>222164</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -6749,7 +6749,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>421362</v>
       </c>
       <c r="E3">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
         <v>43</v>
@@ -6787,7 +6787,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>466695</v>
       </c>
       <c r="E4">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
         <v>46</v>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -6825,7 +6825,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>346674</v>
       </c>
       <c r="E5">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -6863,7 +6863,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -6877,7 +6877,7 @@
         <v>363962</v>
       </c>
       <c r="E6">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
         <v>52</v>
@@ -6901,7 +6901,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>125755</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
         <v>56</v>
@@ -6939,7 +6939,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>150746</v>
       </c>
       <c r="E8">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
         <v>60</v>
@@ -6977,7 +6977,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>145032</v>
       </c>
       <c r="E9">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
         <v>63</v>
@@ -7015,7 +7015,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -7029,7 +7029,7 @@
         <v>161515</v>
       </c>
       <c r="E10">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
         <v>67</v>
@@ -7053,7 +7053,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>109418</v>
       </c>
       <c r="E11">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
         <v>70</v>
@@ -7091,7 +7091,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -7105,7 +7105,7 @@
         <v>96535</v>
       </c>
       <c r="E12">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
         <v>74</v>
@@ -7129,7 +7129,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>100876</v>
       </c>
       <c r="E13">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
         <v>78</v>
@@ -7167,7 +7167,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>103644</v>
       </c>
       <c r="E14">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
         <v>81</v>
@@ -7205,7 +7205,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>106539</v>
       </c>
       <c r="E15">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
         <v>84</v>
@@ -7243,7 +7243,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>99892</v>
       </c>
       <c r="E16">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s">
         <v>88</v>
@@ -7271,7 +7271,7 @@
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -7281,7 +7281,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>85118</v>
       </c>
       <c r="E17">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
         <v>91</v>
@@ -7319,7 +7319,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>92</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>150746</v>
       </c>
       <c r="E18">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
         <v>94</v>
@@ -7357,7 +7357,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>89224</v>
       </c>
       <c r="E19">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
         <v>98</v>
@@ -7395,7 +7395,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>95143</v>
       </c>
       <c r="E20">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
         <v>102</v>
@@ -7433,7 +7433,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>117064</v>
       </c>
       <c r="E21">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
         <v>105</v>
@@ -7471,7 +7471,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>142902</v>
       </c>
       <c r="E22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
         <v>109</v>
@@ -7509,7 +7509,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>110</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>162945</v>
       </c>
       <c r="E23">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F23" t="s">
         <v>112</v>
@@ -7547,7 +7547,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>170602</v>
       </c>
       <c r="E24">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
         <v>116</v>
@@ -7575,7 +7575,7 @@
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -7585,7 +7585,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -7599,7 +7599,7 @@
         <v>124914</v>
       </c>
       <c r="E25">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
         <v>119</v>
@@ -7623,7 +7623,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>75304</v>
       </c>
       <c r="E26">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
         <v>123</v>
@@ -7661,7 +7661,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>124</v>
       </c>
@@ -7675,7 +7675,7 @@
         <v>104885</v>
       </c>
       <c r="E27">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
         <v>126</v>
@@ -7689,7 +7689,7 @@
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -7699,7 +7699,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>142702</v>
       </c>
       <c r="E28">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
         <v>129</v>
@@ -7737,7 +7737,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>130</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>265589</v>
       </c>
       <c r="E29">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F29" t="s">
         <v>133</v>
@@ -7775,7 +7775,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>155074</v>
       </c>
       <c r="E30">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F30" t="s">
         <v>137</v>
@@ -7813,7 +7813,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>138</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>90643</v>
       </c>
       <c r="E31">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
         <v>141</v>
@@ -7841,7 +7841,7 @@
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -7851,7 +7851,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>142</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>100024</v>
       </c>
       <c r="E32">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F32" t="s">
         <v>145</v>
@@ -7879,7 +7879,7 @@
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -7889,7 +7889,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>146</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>94202</v>
       </c>
       <c r="E33">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F33" t="s">
         <v>148</v>
@@ -7917,7 +7917,7 @@
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -7927,7 +7927,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>136756</v>
       </c>
       <c r="E34">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F34" t="s">
         <v>151</v>
@@ -7965,7 +7965,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>152</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>126502</v>
       </c>
       <c r="E35">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F35" t="s">
         <v>153</v>
@@ -7993,7 +7993,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -8003,7 +8003,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>154</v>
       </c>
@@ -8017,7 +8017,7 @@
         <v>95031</v>
       </c>
       <c r="E36">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
         <v>156</v>
@@ -8041,7 +8041,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>153995</v>
       </c>
       <c r="E37">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F37" t="s">
         <v>160</v>
@@ -8069,7 +8069,7 @@
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K37">
         <v>1</v>
@@ -8079,7 +8079,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -8093,7 +8093,7 @@
         <v>175837</v>
       </c>
       <c r="E38">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F38" t="s">
         <v>164</v>
@@ -8117,7 +8117,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -8131,7 +8131,7 @@
         <v>119817</v>
       </c>
       <c r="E39">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F39" t="s">
         <v>168</v>
@@ -8155,7 +8155,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>130295</v>
       </c>
       <c r="E40">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F40" t="s">
         <v>172</v>
@@ -8193,7 +8193,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>173</v>
       </c>
@@ -8207,7 +8207,7 @@
         <v>152716</v>
       </c>
       <c r="E41">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F41" t="s">
         <v>175</v>
@@ -8231,7 +8231,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>176</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>101865</v>
       </c>
       <c r="E42">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F42" t="s">
         <v>178</v>
@@ -8269,7 +8269,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>179</v>
       </c>
@@ -8283,7 +8283,7 @@
         <v>156190</v>
       </c>
       <c r="E43">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F43" t="s">
         <v>182</v>
@@ -8307,7 +8307,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>183</v>
       </c>
@@ -8321,7 +8321,7 @@
         <v>150916</v>
       </c>
       <c r="E44">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s">
         <v>186</v>
@@ -8345,7 +8345,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>187</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>150916</v>
       </c>
       <c r="E45">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F45" t="s">
         <v>188</v>
@@ -8383,7 +8383,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>189</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>92751</v>
       </c>
       <c r="E46">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s">
         <v>192</v>
@@ -8411,7 +8411,7 @@
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K46">
         <v>1</v>
@@ -8421,7 +8421,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>193</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>108571</v>
       </c>
       <c r="E47">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F47" t="s">
         <v>195</v>
@@ -8449,7 +8449,7 @@
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -8459,7 +8459,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>196</v>
       </c>
@@ -8473,7 +8473,7 @@
         <v>95020</v>
       </c>
       <c r="E48">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F48" t="s">
         <v>199</v>
@@ -8497,7 +8497,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>200</v>
       </c>
@@ -8511,7 +8511,7 @@
         <v>115578</v>
       </c>
       <c r="E49">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F49" t="s">
         <v>202</v>
@@ -8535,7 +8535,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>203</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>135583</v>
       </c>
       <c r="E50">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F50" t="s">
         <v>206</v>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K50">
         <v>1</v>
@@ -8573,7 +8573,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>207</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>145312</v>
       </c>
       <c r="E51">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F51" t="s">
         <v>209</v>
@@ -8611,7 +8611,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>210</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>131886</v>
       </c>
       <c r="E52">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F52" t="s">
         <v>212</v>
@@ -8649,7 +8649,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>213</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>143990</v>
       </c>
       <c r="E53">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F53" t="s">
         <v>214</v>
@@ -8687,7 +8687,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>215</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>463706</v>
       </c>
       <c r="E54">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F54" t="s">
         <v>217</v>
@@ -8725,7 +8725,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>218</v>
       </c>
@@ -8739,7 +8739,7 @@
         <v>109513</v>
       </c>
       <c r="E55">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F55" t="s">
         <v>220</v>
@@ -8763,7 +8763,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>221</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>139155</v>
       </c>
       <c r="E56">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F56" t="s">
         <v>223</v>
@@ -8801,7 +8801,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>224</v>
       </c>
@@ -8815,7 +8815,7 @@
         <v>100620</v>
       </c>
       <c r="E57">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F57" t="s">
         <v>226</v>
@@ -8839,7 +8839,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>227</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>93150</v>
       </c>
       <c r="E58">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F58" t="s">
         <v>228</v>
@@ -8877,7 +8877,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>229</v>
       </c>
@@ -8891,7 +8891,7 @@
         <v>144060</v>
       </c>
       <c r="E59">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F59" t="s">
         <v>230</v>
@@ -8915,7 +8915,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>231</v>
       </c>
@@ -8929,7 +8929,7 @@
         <v>132894</v>
       </c>
       <c r="E60">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F60" t="s">
         <v>234</v>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K60">
         <v>1</v>
@@ -8953,7 +8953,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>235</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>94582</v>
       </c>
       <c r="E61">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F61" t="s">
         <v>237</v>
@@ -8991,7 +8991,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>238</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>110395</v>
       </c>
       <c r="E62">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F62" t="s">
         <v>240</v>
@@ -9029,7 +9029,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>241</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>113582</v>
       </c>
       <c r="E63">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F63" t="s">
         <v>243</v>
@@ -9067,7 +9067,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>244</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>86539</v>
       </c>
       <c r="E64">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F64" t="s">
         <v>245</v>
@@ -9105,7 +9105,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>246</v>
       </c>
@@ -9119,7 +9119,7 @@
         <v>129232</v>
       </c>
       <c r="E65">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F65" t="s">
         <v>247</v>
@@ -9143,7 +9143,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>248</v>
       </c>
@@ -9157,7 +9157,7 @@
         <v>120701</v>
       </c>
       <c r="E66">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F66" t="s">
         <v>249</v>
@@ -9181,7 +9181,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>250</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>112938</v>
       </c>
       <c r="E67">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F67" t="s">
         <v>251</v>
@@ -9219,7 +9219,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>252</v>
       </c>
@@ -9233,7 +9233,7 @@
         <v>135222</v>
       </c>
       <c r="E68">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F68" t="s">
         <v>254</v>
@@ -9257,7 +9257,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>255</v>
       </c>
@@ -9271,7 +9271,7 @@
         <v>122970</v>
       </c>
       <c r="E69">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F69" t="s">
         <v>257</v>
@@ -9285,7 +9285,7 @@
       </c>
       <c r="J69">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -9295,7 +9295,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>258</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>119580</v>
       </c>
       <c r="E70">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F70" t="s">
         <v>260</v>
@@ -9333,7 +9333,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>261</v>
       </c>
@@ -9347,7 +9347,7 @@
         <v>124086</v>
       </c>
       <c r="E71">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F71" t="s">
         <v>264</v>
@@ -9371,7 +9371,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>265</v>
       </c>
@@ -9385,7 +9385,7 @@
         <v>131886</v>
       </c>
       <c r="E72">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F72" t="s">
         <v>266</v>
@@ -9409,7 +9409,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>267</v>
       </c>
@@ -9423,7 +9423,7 @@
         <v>126549</v>
       </c>
       <c r="E73">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F73" t="s">
         <v>270</v>
@@ -9437,7 +9437,7 @@
       </c>
       <c r="J73">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -9447,7 +9447,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>271</v>
       </c>
@@ -9461,7 +9461,7 @@
         <v>142277</v>
       </c>
       <c r="E74">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F74" t="s">
         <v>273</v>
@@ -9485,7 +9485,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>274</v>
       </c>
@@ -9496,10 +9496,10 @@
         <v>276</v>
       </c>
       <c r="D75">
-        <v>116987</v>
+        <v>115258</v>
       </c>
       <c r="E75">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F75" t="s">
         <v>277</v>
@@ -9513,7 +9513,7 @@
       </c>
       <c r="J75">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K75">
         <v>1</v>
@@ -9523,7 +9523,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>278</v>
       </c>
@@ -9537,7 +9537,7 @@
         <v>172214</v>
       </c>
       <c r="E76">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F76" t="s">
         <v>281</v>
@@ -9561,7 +9561,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>282</v>
       </c>
@@ -9575,7 +9575,7 @@
         <v>1765255</v>
       </c>
       <c r="E77">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F77" t="s">
         <v>285</v>
@@ -9599,7 +9599,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>286</v>
       </c>
@@ -9613,7 +9613,7 @@
         <v>1116026</v>
       </c>
       <c r="E78">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F78" t="s">
         <v>288</v>
@@ -9637,7 +9637,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>289</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>240902</v>
       </c>
       <c r="E79">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F79" t="s">
         <v>291</v>
@@ -9675,7 +9675,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>292</v>
       </c>
@@ -9689,7 +9689,7 @@
         <v>155859</v>
       </c>
       <c r="E80">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F80" t="s">
         <v>294</v>
@@ -9713,7 +9713,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>295</v>
       </c>
@@ -9727,7 +9727,7 @@
         <v>70947</v>
       </c>
       <c r="E81">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F81" t="s">
         <v>298</v>
@@ -9751,7 +9751,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>299</v>
       </c>
@@ -9765,7 +9765,7 @@
         <v>157707</v>
       </c>
       <c r="E82">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F82" t="s">
         <v>302</v>
@@ -9789,7 +9789,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>303</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>135323</v>
       </c>
       <c r="E83">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F83" t="s">
         <v>306</v>
@@ -9827,7 +9827,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>307</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>108000</v>
       </c>
       <c r="E84">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F84" t="s">
         <v>310</v>
@@ -9865,7 +9865,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>311</v>
       </c>
@@ -9879,7 +9879,7 @@
         <v>80275</v>
       </c>
       <c r="E85">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F85" t="s">
         <v>314</v>
@@ -9903,7 +9903,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>315</v>
       </c>
@@ -9917,7 +9917,7 @@
         <v>140290</v>
       </c>
       <c r="E86">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F86" t="s">
         <v>317</v>
@@ -9941,7 +9941,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>318</v>
       </c>
@@ -9955,7 +9955,7 @@
         <v>133838</v>
       </c>
       <c r="E87">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F87" t="s">
         <v>320</v>
@@ -9969,7 +9969,7 @@
       </c>
       <c r="J87">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K87">
         <v>1</v>
@@ -9979,7 +9979,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>321</v>
       </c>
@@ -9993,7 +9993,7 @@
         <v>177565</v>
       </c>
       <c r="E88">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F88" t="s">
         <v>322</v>
@@ -10017,7 +10017,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>323</v>
       </c>
@@ -10031,7 +10031,7 @@
         <v>170724</v>
       </c>
       <c r="E89">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F89" t="s">
         <v>325</v>
@@ -10055,7 +10055,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>326</v>
       </c>
@@ -10069,7 +10069,7 @@
         <v>147957</v>
       </c>
       <c r="E90">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F90" t="s">
         <v>328</v>
@@ -10083,7 +10083,7 @@
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -10093,7 +10093,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>329</v>
       </c>
@@ -10107,7 +10107,7 @@
         <v>146911</v>
       </c>
       <c r="E91">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F91" t="s">
         <v>330</v>
@@ -10131,7 +10131,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>331</v>
       </c>
@@ -10145,7 +10145,7 @@
         <v>151160</v>
       </c>
       <c r="E92">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F92" t="s">
         <v>334</v>
@@ -10169,7 +10169,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>335</v>
       </c>
@@ -10183,7 +10183,7 @@
         <v>129060</v>
       </c>
       <c r="E93">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F93" t="s">
         <v>338</v>
@@ -10207,7 +10207,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>339</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>162422</v>
       </c>
       <c r="E94">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F94" t="s">
         <v>341</v>
@@ -10245,7 +10245,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>342</v>
       </c>
@@ -10259,7 +10259,7 @@
         <v>93478</v>
       </c>
       <c r="E95">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F95" t="s">
         <v>345</v>
@@ -10273,7 +10273,7 @@
       </c>
       <c r="J95">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -10283,7 +10283,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>346</v>
       </c>
@@ -10297,7 +10297,7 @@
         <v>74233</v>
       </c>
       <c r="E96">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F96" t="s">
         <v>349</v>
@@ -10321,7 +10321,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>350</v>
       </c>
@@ -10335,7 +10335,7 @@
         <v>58000</v>
       </c>
       <c r="E97">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F97" t="s">
         <v>352</v>
@@ -10359,7 +10359,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>353</v>
       </c>
@@ -10373,7 +10373,7 @@
         <v>92562</v>
       </c>
       <c r="E98">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F98" t="s">
         <v>355</v>
@@ -10397,7 +10397,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>356</v>
       </c>
@@ -10411,7 +10411,7 @@
         <v>79811</v>
       </c>
       <c r="E99">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F99" t="s">
         <v>357</v>
@@ -10435,7 +10435,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>358</v>
       </c>
@@ -10449,7 +10449,7 @@
         <v>72179</v>
       </c>
       <c r="E100">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F100" t="s">
         <v>359</v>
@@ -10473,7 +10473,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>360</v>
       </c>
@@ -10487,7 +10487,7 @@
         <v>93478</v>
       </c>
       <c r="E101">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F101" t="s">
         <v>362</v>
@@ -10525,13 +10525,13 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -10539,7 +10539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -10555,7 +10555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -10571,7 +10571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -10579,7 +10579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -10587,7 +10587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -10611,7 +10611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -10635,7 +10635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -10643,7 +10643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -10659,7 +10659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -10667,7 +10667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -10675,7 +10675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>

</xml_diff>